<commit_message>
Moved column saver to use matlab code.
</commit_message>
<xml_diff>
--- a/scilab/datahandling/project_description.xlsx
+++ b/scilab/datahandling/project_description.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="instron_tracking" sheetId="1" r:id="rId1"/>
@@ -685,8 +685,6 @@
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -694,27 +692,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -722,15 +722,15 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1339,310 +1339,310 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="3"/>
-    <col min="2" max="2" width="19.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="17.33203125" style="3"/>
-    <col min="6" max="6" width="19" style="3" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="17.33203125" style="3"/>
+    <col min="1" max="1" width="17.33203125" style="1"/>
+    <col min="2" max="2" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="17.33203125" style="1"/>
+    <col min="6" max="6" width="19" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="17.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" thickBot="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="16" thickTop="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="16" thickBot="1">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" ht="16" thickTop="1">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="11" t="s">
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="13">
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="13">
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="13">
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="13">
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="13">
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="13">
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="13">
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="13">
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="9">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="13">
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" thickBot="1">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
     </row>
     <row r="20" spans="1:10" ht="16" thickTop="1">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14" t="s">
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" ht="16" thickBot="1">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="15" t="s">
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="10" t="s">
         <v>46</v>
       </c>
       <c r="I21" s="18" t="s">
@@ -1651,131 +1651,137 @@
       <c r="J21" s="19"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="13" t="s">
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I22" s="22" t="s">
+      <c r="I22" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="J22" s="22"/>
+      <c r="J22" s="17"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="13" t="s">
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I23" s="22" t="s">
+      <c r="I23" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="22"/>
+      <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
@@ -1787,17 +1793,11 @@
     <mergeCell ref="D20:G20"/>
     <mergeCell ref="A19:J19"/>
     <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>